<commit_message>
Modificacion de archivos proyecto y seguridad
</commit_message>
<xml_diff>
--- a/Documentacion/Proyecto/Cronograma JANFOX.xlsx
+++ b/Documentacion/Proyecto/Cronograma JANFOX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\Videojuego\JanFox_V2\Documentacion\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF083C6-FBA0-4B92-8F30-074A6743C911}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080503B3-D6A7-416E-8AFB-15A85D6FF030}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma general" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,26 @@
     <sheet name="Sprint 5" sheetId="11" r:id="rId8"/>
     <sheet name="Sprint 6" sheetId="12" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="137">
   <si>
     <t>Completado</t>
   </si>
@@ -445,6 +454,9 @@
   </si>
   <si>
     <t>Andres, Natalia y Janel</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
 </sst>
 </file>
@@ -1716,10 +1728,41 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1764,25 +1807,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1791,22 +1816,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4277,8 +4287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:QO94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4441,20 +4451,20 @@
       <c r="E3" s="76"/>
       <c r="F3" s="76"/>
       <c r="G3" s="86"/>
-      <c r="H3" s="195" t="s">
+      <c r="H3" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="195"/>
+      <c r="I3" s="185"/>
       <c r="J3" s="69"/>
-      <c r="K3" s="195" t="s">
+      <c r="K3" s="185" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="195"/>
+      <c r="L3" s="185"/>
       <c r="M3" s="72"/>
-      <c r="N3" s="196" t="s">
+      <c r="N3" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="196"/>
+      <c r="O3" s="185"/>
       <c r="P3" s="62"/>
       <c r="BX3" s="79"/>
       <c r="BY3" s="80"/>
@@ -4515,10 +4525,10 @@
     </row>
     <row r="5" spans="1:457" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="201" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="188" t="s">
+      <c r="C5" s="199" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="68" t="s">
@@ -4527,114 +4537,114 @@
       <c r="E5" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="186" t="s">
+      <c r="F5" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="184" t="s">
+      <c r="G5" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="183" t="s">
+      <c r="H5" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="179"/>
-      <c r="J5" s="179"/>
-      <c r="K5" s="179"/>
-      <c r="L5" s="179" t="s">
+      <c r="I5" s="188"/>
+      <c r="J5" s="188"/>
+      <c r="K5" s="188"/>
+      <c r="L5" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="179"/>
-      <c r="N5" s="179"/>
-      <c r="O5" s="179"/>
-      <c r="P5" s="179" t="s">
+      <c r="M5" s="188"/>
+      <c r="N5" s="188"/>
+      <c r="O5" s="188"/>
+      <c r="P5" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="Q5" s="179"/>
-      <c r="R5" s="179"/>
-      <c r="S5" s="179"/>
-      <c r="T5" s="179" t="s">
+      <c r="Q5" s="188"/>
+      <c r="R5" s="188"/>
+      <c r="S5" s="188"/>
+      <c r="T5" s="188" t="s">
         <v>12</v>
       </c>
-      <c r="U5" s="179"/>
-      <c r="V5" s="179"/>
-      <c r="W5" s="179"/>
-      <c r="X5" s="179" t="s">
+      <c r="U5" s="188"/>
+      <c r="V5" s="188"/>
+      <c r="W5" s="188"/>
+      <c r="X5" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="Y5" s="179"/>
-      <c r="Z5" s="179"/>
-      <c r="AA5" s="179"/>
-      <c r="AB5" s="179" t="s">
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
+      <c r="AB5" s="188" t="s">
         <v>14</v>
       </c>
-      <c r="AC5" s="179"/>
-      <c r="AD5" s="179"/>
-      <c r="AE5" s="179"/>
-      <c r="AF5" s="179" t="s">
+      <c r="AC5" s="188"/>
+      <c r="AD5" s="188"/>
+      <c r="AE5" s="188"/>
+      <c r="AF5" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="AG5" s="179"/>
-      <c r="AH5" s="179"/>
-      <c r="AI5" s="179"/>
-      <c r="AJ5" s="179" t="s">
+      <c r="AG5" s="188"/>
+      <c r="AH5" s="188"/>
+      <c r="AI5" s="188"/>
+      <c r="AJ5" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="AK5" s="179"/>
-      <c r="AL5" s="179"/>
-      <c r="AM5" s="179"/>
-      <c r="AN5" s="179" t="s">
+      <c r="AK5" s="188"/>
+      <c r="AL5" s="188"/>
+      <c r="AM5" s="188"/>
+      <c r="AN5" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="AO5" s="179"/>
-      <c r="AP5" s="179"/>
-      <c r="AQ5" s="179"/>
-      <c r="AR5" s="179" t="s">
+      <c r="AO5" s="188"/>
+      <c r="AP5" s="188"/>
+      <c r="AQ5" s="188"/>
+      <c r="AR5" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="AS5" s="179"/>
-      <c r="AT5" s="179"/>
-      <c r="AU5" s="179"/>
-      <c r="AV5" s="179" t="s">
+      <c r="AS5" s="188"/>
+      <c r="AT5" s="188"/>
+      <c r="AU5" s="188"/>
+      <c r="AV5" s="188" t="s">
         <v>19</v>
       </c>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="179"/>
-      <c r="AY5" s="179"/>
-      <c r="AZ5" s="179" t="s">
+      <c r="AW5" s="188"/>
+      <c r="AX5" s="188"/>
+      <c r="AY5" s="188"/>
+      <c r="AZ5" s="188" t="s">
         <v>20</v>
       </c>
-      <c r="BA5" s="179"/>
-      <c r="BB5" s="179"/>
-      <c r="BC5" s="179"/>
-      <c r="BD5" s="179" t="s">
+      <c r="BA5" s="188"/>
+      <c r="BB5" s="188"/>
+      <c r="BC5" s="188"/>
+      <c r="BD5" s="188" t="s">
         <v>21</v>
       </c>
-      <c r="BE5" s="179"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BH5" s="179" t="s">
+      <c r="BE5" s="188"/>
+      <c r="BF5" s="188"/>
+      <c r="BG5" s="188"/>
+      <c r="BH5" s="188" t="s">
         <v>22</v>
       </c>
-      <c r="BI5" s="179"/>
-      <c r="BJ5" s="179"/>
-      <c r="BK5" s="179"/>
-      <c r="BL5" s="179" t="s">
+      <c r="BI5" s="188"/>
+      <c r="BJ5" s="188"/>
+      <c r="BK5" s="188"/>
+      <c r="BL5" s="188" t="s">
         <v>23</v>
       </c>
-      <c r="BM5" s="179"/>
-      <c r="BN5" s="179"/>
-      <c r="BO5" s="179"/>
-      <c r="BP5" s="179" t="s">
+      <c r="BM5" s="188"/>
+      <c r="BN5" s="188"/>
+      <c r="BO5" s="188"/>
+      <c r="BP5" s="188" t="s">
         <v>24</v>
       </c>
-      <c r="BQ5" s="179"/>
-      <c r="BR5" s="179"/>
-      <c r="BS5" s="179"/>
-      <c r="BT5" s="179" t="s">
+      <c r="BQ5" s="188"/>
+      <c r="BR5" s="188"/>
+      <c r="BS5" s="188"/>
+      <c r="BT5" s="188" t="s">
         <v>25</v>
       </c>
-      <c r="BU5" s="179"/>
-      <c r="BV5" s="179"/>
-      <c r="BW5" s="180"/>
+      <c r="BU5" s="188"/>
+      <c r="BV5" s="188"/>
+      <c r="BW5" s="206"/>
       <c r="BX5" s="56"/>
       <c r="BY5" s="53"/>
       <c r="BZ5" s="53"/>
@@ -5020,12 +5030,12 @@
     </row>
     <row r="6" spans="1:457" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
-      <c r="B6" s="191"/>
-      <c r="C6" s="189"/>
+      <c r="B6" s="202"/>
+      <c r="C6" s="200"/>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="185"/>
+      <c r="F6" s="198"/>
+      <c r="G6" s="196"/>
       <c r="H6" s="51" t="s">
         <v>26</v>
       </c>
@@ -5255,7 +5265,7 @@
     </row>
     <row r="7" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
-      <c r="B7" s="199" t="s">
+      <c r="B7" s="189" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="33" t="s">
@@ -5700,7 +5710,7 @@
     </row>
     <row r="8" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
-      <c r="B8" s="200"/>
+      <c r="B8" s="190"/>
       <c r="C8" s="5" t="s">
         <v>34</v>
       </c>
@@ -6143,7 +6153,7 @@
     </row>
     <row r="9" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
-      <c r="B9" s="201" t="s">
+      <c r="B9" s="191" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -6588,7 +6598,7 @@
     </row>
     <row r="10" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
-      <c r="B10" s="181"/>
+      <c r="B10" s="192"/>
       <c r="C10" s="5" t="s">
         <v>39</v>
       </c>
@@ -7031,7 +7041,7 @@
     </row>
     <row r="11" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
-      <c r="B11" s="181"/>
+      <c r="B11" s="192"/>
       <c r="C11" s="5" t="s">
         <v>40</v>
       </c>
@@ -7474,7 +7484,7 @@
     </row>
     <row r="12" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
-      <c r="B12" s="181"/>
+      <c r="B12" s="192"/>
       <c r="C12" s="5" t="s">
         <v>41</v>
       </c>
@@ -7917,7 +7927,7 @@
     </row>
     <row r="13" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
-      <c r="B13" s="181"/>
+      <c r="B13" s="192"/>
       <c r="C13" s="5" t="s">
         <v>42</v>
       </c>
@@ -8360,7 +8370,7 @@
     </row>
     <row r="14" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
-      <c r="B14" s="181"/>
+      <c r="B14" s="192"/>
       <c r="C14" s="5" t="s">
         <v>43</v>
       </c>
@@ -8803,7 +8813,7 @@
     </row>
     <row r="15" spans="1:457" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
-      <c r="B15" s="197" t="s">
+      <c r="B15" s="186" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="48" t="s">
@@ -9248,7 +9258,7 @@
     </row>
     <row r="16" spans="1:457" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
-      <c r="B16" s="198"/>
+      <c r="B16" s="187"/>
       <c r="C16" s="48" t="s">
         <v>47</v>
       </c>
@@ -9687,7 +9697,7 @@
     </row>
     <row r="17" spans="1:452" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
-      <c r="B17" s="192" t="s">
+      <c r="B17" s="203" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="48" t="s">
@@ -10128,7 +10138,7 @@
     </row>
     <row r="18" spans="1:452" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
-      <c r="B18" s="193"/>
+      <c r="B18" s="204"/>
       <c r="C18" s="49" t="s">
         <v>50</v>
       </c>
@@ -10571,7 +10581,7 @@
     </row>
     <row r="19" spans="1:452" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
-      <c r="B19" s="193"/>
+      <c r="B19" s="204"/>
       <c r="C19" s="49" t="s">
         <v>51</v>
       </c>
@@ -11010,7 +11020,7 @@
     </row>
     <row r="20" spans="1:452" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
-      <c r="B20" s="193"/>
+      <c r="B20" s="204"/>
       <c r="C20" s="49" t="s">
         <v>119</v>
       </c>
@@ -11449,7 +11459,7 @@
     </row>
     <row r="21" spans="1:452" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
-      <c r="B21" s="193"/>
+      <c r="B21" s="204"/>
       <c r="C21" s="49" t="s">
         <v>55</v>
       </c>
@@ -11888,7 +11898,7 @@
     </row>
     <row r="22" spans="1:452" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
-      <c r="B22" s="194"/>
+      <c r="B22" s="205"/>
       <c r="C22" s="49" t="s">
         <v>56</v>
       </c>
@@ -12327,7 +12337,7 @@
     </row>
     <row r="23" spans="1:452" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
-      <c r="B23" s="181" t="s">
+      <c r="B23" s="192" t="s">
         <v>57</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -12772,7 +12782,7 @@
     </row>
     <row r="24" spans="1:452" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
-      <c r="B24" s="181"/>
+      <c r="B24" s="192"/>
       <c r="C24" s="9" t="s">
         <v>59</v>
       </c>
@@ -13209,15 +13219,15 @@
       <c r="QI24" s="4"/>
       <c r="QJ24" s="4"/>
     </row>
-    <row r="25" spans="1:452" s="209" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="204"/>
-      <c r="B25" s="182"/>
+    <row r="25" spans="1:452" s="184" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="179"/>
+      <c r="B25" s="193"/>
       <c r="C25" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="205" t="s">
+      <c r="F25" s="180" t="s">
         <v>61</v>
       </c>
       <c r="G25" s="88" t="s">
@@ -13290,29 +13300,29 @@
       <c r="BT25" s="119"/>
       <c r="BU25" s="119"/>
       <c r="BV25" s="119"/>
-      <c r="BW25" s="206"/>
-      <c r="BX25" s="207"/>
-      <c r="BY25" s="208"/>
-      <c r="BZ25" s="208"/>
-      <c r="CA25" s="208"/>
-      <c r="CB25" s="208"/>
-      <c r="CC25" s="208"/>
-      <c r="CD25" s="208"/>
-      <c r="CE25" s="208"/>
-      <c r="CF25" s="208"/>
-      <c r="CG25" s="208"/>
-      <c r="CH25" s="208"/>
-      <c r="CI25" s="208"/>
-      <c r="CJ25" s="208"/>
-      <c r="CK25" s="208"/>
-      <c r="CL25" s="208"/>
-      <c r="CM25" s="208"/>
-      <c r="CN25" s="208"/>
-      <c r="CO25" s="208"/>
-      <c r="CP25" s="208"/>
-      <c r="CQ25" s="208"/>
-      <c r="CR25" s="208"/>
-      <c r="CS25" s="208"/>
+      <c r="BW25" s="181"/>
+      <c r="BX25" s="182"/>
+      <c r="BY25" s="183"/>
+      <c r="BZ25" s="183"/>
+      <c r="CA25" s="183"/>
+      <c r="CB25" s="183"/>
+      <c r="CC25" s="183"/>
+      <c r="CD25" s="183"/>
+      <c r="CE25" s="183"/>
+      <c r="CF25" s="183"/>
+      <c r="CG25" s="183"/>
+      <c r="CH25" s="183"/>
+      <c r="CI25" s="183"/>
+      <c r="CJ25" s="183"/>
+      <c r="CK25" s="183"/>
+      <c r="CL25" s="183"/>
+      <c r="CM25" s="183"/>
+      <c r="CN25" s="183"/>
+      <c r="CO25" s="183"/>
+      <c r="CP25" s="183"/>
+      <c r="CQ25" s="183"/>
+      <c r="CR25" s="183"/>
+      <c r="CS25" s="183"/>
       <c r="CT25" s="119"/>
       <c r="CU25" s="119"/>
       <c r="CV25" s="119"/>
@@ -17471,18 +17481,14 @@
     <row r="35" spans="1:452" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="16" t="s">
-        <v>53</v>
-      </c>
+      <c r="C35" s="16"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="91"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
-      <c r="J35" s="126">
-        <v>44272</v>
-      </c>
+      <c r="J35" s="126"/>
       <c r="K35" s="11"/>
       <c r="L35" s="11"/>
       <c r="M35" s="11"/>
@@ -17538,18 +17544,14 @@
     <row r="36" spans="1:452" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="12"/>
-      <c r="C36" s="16" t="s">
-        <v>131</v>
-      </c>
+      <c r="C36" s="16"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="91"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
-      <c r="J36" s="126">
-        <v>44272</v>
-      </c>
+      <c r="J36" s="126"/>
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
       <c r="M36" s="11"/>
@@ -17604,20 +17606,13 @@
     </row>
     <row r="37" spans="1:452" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
-      <c r="C37" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="91"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="126">
-        <v>44273</v>
-      </c>
-      <c r="J37" s="126">
-        <v>44282</v>
-      </c>
+      <c r="I37" s="126"/>
+      <c r="J37" s="126"/>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
@@ -17671,15 +17666,13 @@
       <c r="BW37" s="55"/>
     </row>
     <row r="38" spans="1:452" x14ac:dyDescent="0.25">
-      <c r="C38" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I38" s="126">
-        <v>44273</v>
-      </c>
-      <c r="J38" s="126">
-        <v>44282</v>
-      </c>
+      <c r="B38" s="73"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="I38" s="126"/>
+      <c r="J38" s="126"/>
       <c r="AN38" s="19"/>
       <c r="AO38" s="52"/>
       <c r="AP38" s="52"/>
@@ -17718,15 +17711,13 @@
       <c r="BW38" s="55"/>
     </row>
     <row r="39" spans="1:452" x14ac:dyDescent="0.25">
-      <c r="C39" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="125">
-        <v>44256</v>
-      </c>
-      <c r="J39" s="125">
-        <v>44261</v>
-      </c>
+      <c r="B39" s="73"/>
+      <c r="C39" s="209"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="I39" s="125"/>
+      <c r="J39" s="125"/>
       <c r="AN39" s="19"/>
       <c r="AO39" s="52"/>
       <c r="AP39" s="52"/>
@@ -17765,15 +17756,13 @@
       <c r="BW39" s="55"/>
     </row>
     <row r="40" spans="1:452" x14ac:dyDescent="0.25">
-      <c r="C40" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I40" s="125">
-        <v>44263</v>
-      </c>
-      <c r="J40" s="125">
-        <v>44268</v>
-      </c>
+      <c r="B40" s="73"/>
+      <c r="C40" s="209"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="I40" s="125"/>
+      <c r="J40" s="125"/>
       <c r="AN40" s="19"/>
       <c r="AO40" s="52"/>
       <c r="AP40" s="52"/>
@@ -17812,15 +17801,13 @@
       <c r="BW40" s="55"/>
     </row>
     <row r="41" spans="1:452" x14ac:dyDescent="0.25">
-      <c r="C41" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="125">
-        <v>44270</v>
-      </c>
-      <c r="J41" s="125">
-        <v>44282</v>
-      </c>
+      <c r="B41" s="73"/>
+      <c r="C41" s="209"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="I41" s="125"/>
+      <c r="J41" s="125"/>
       <c r="AN41" s="19"/>
       <c r="AO41" s="52"/>
       <c r="AP41" s="52"/>
@@ -17859,15 +17846,13 @@
       <c r="BW41" s="55"/>
     </row>
     <row r="42" spans="1:452" x14ac:dyDescent="0.25">
-      <c r="C42" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I42" s="125">
-        <v>44270</v>
-      </c>
-      <c r="J42" s="125">
-        <v>44282</v>
-      </c>
+      <c r="B42" s="73"/>
+      <c r="C42" s="209"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="I42" s="125"/>
+      <c r="J42" s="125"/>
       <c r="AN42" s="19"/>
       <c r="AO42" s="52"/>
       <c r="AP42" s="52"/>
@@ -17906,15 +17891,13 @@
       <c r="BW42" s="55"/>
     </row>
     <row r="43" spans="1:452" x14ac:dyDescent="0.25">
-      <c r="C43" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I43" s="125">
-        <v>44291</v>
-      </c>
-      <c r="J43" s="125">
-        <v>44296</v>
-      </c>
+      <c r="B43" s="73"/>
+      <c r="C43" s="209"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="I43" s="125"/>
+      <c r="J43" s="125"/>
       <c r="AN43" s="19"/>
       <c r="AO43" s="52"/>
       <c r="AP43" s="52"/>
@@ -17953,13 +17936,13 @@
       <c r="BW43" s="55"/>
     </row>
     <row r="44" spans="1:452" x14ac:dyDescent="0.25">
-      <c r="C44" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B44" s="73"/>
+      <c r="C44" s="74"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
       <c r="G44" s="122"/>
-      <c r="J44" s="125">
-        <v>44303</v>
-      </c>
+      <c r="J44" s="125"/>
       <c r="AN44" s="19"/>
       <c r="AO44" s="52"/>
       <c r="AP44" s="52"/>
@@ -17997,16 +17980,9 @@
       <c r="BV44" s="52"/>
       <c r="BW44" s="55"/>
     </row>
-    <row r="45" spans="1:452" ht="24" x14ac:dyDescent="0.25">
-      <c r="C45" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J45" s="125">
-        <v>44303</v>
-      </c>
-      <c r="K45" s="124">
-        <v>0.9</v>
-      </c>
+    <row r="45" spans="1:452" x14ac:dyDescent="0.25">
+      <c r="J45" s="125"/>
+      <c r="K45" s="124"/>
       <c r="AN45" s="19"/>
       <c r="AO45" s="52"/>
       <c r="AP45" s="52"/>
@@ -18045,13 +18021,8 @@
       <c r="BW45" s="55"/>
     </row>
     <row r="46" spans="1:452" x14ac:dyDescent="0.25">
-      <c r="C46" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G46" s="122"/>
-      <c r="J46" s="125">
-        <v>44303</v>
-      </c>
+      <c r="J46" s="125"/>
       <c r="AN46" s="19"/>
       <c r="AO46" s="52"/>
       <c r="AP46" s="52"/>
@@ -18165,10 +18136,8 @@
       <c r="BV48" s="52"/>
       <c r="BW48" s="55"/>
     </row>
-    <row r="49" spans="9:75" ht="24" x14ac:dyDescent="0.25">
-      <c r="K49" s="124">
-        <v>0.2</v>
-      </c>
+    <row r="49" spans="9:75" x14ac:dyDescent="0.25">
+      <c r="K49" s="124"/>
       <c r="AN49" s="19"/>
       <c r="AO49" s="52"/>
       <c r="AP49" s="52"/>
@@ -18206,10 +18175,8 @@
       <c r="BV49" s="52"/>
       <c r="BW49" s="55"/>
     </row>
-    <row r="50" spans="9:75" ht="24" x14ac:dyDescent="0.25">
-      <c r="K50" s="124">
-        <v>0.2</v>
-      </c>
+    <row r="50" spans="9:75" x14ac:dyDescent="0.25">
+      <c r="K50" s="124"/>
       <c r="AN50" s="19"/>
       <c r="AO50" s="52"/>
       <c r="AP50" s="52"/>
@@ -18247,10 +18214,8 @@
       <c r="BV50" s="52"/>
       <c r="BW50" s="55"/>
     </row>
-    <row r="51" spans="9:75" ht="24" x14ac:dyDescent="0.25">
-      <c r="K51" s="124">
-        <v>0.2</v>
-      </c>
+    <row r="51" spans="9:75" x14ac:dyDescent="0.25">
+      <c r="K51" s="124"/>
       <c r="AN51" s="19"/>
       <c r="AO51" s="52"/>
       <c r="AP51" s="52"/>
@@ -18288,16 +18253,10 @@
       <c r="BV51" s="52"/>
       <c r="BW51" s="55"/>
     </row>
-    <row r="52" spans="9:75" ht="24" x14ac:dyDescent="0.25">
-      <c r="I52" s="125">
-        <v>44291</v>
-      </c>
-      <c r="J52" s="125">
-        <v>44303</v>
-      </c>
-      <c r="K52" s="124">
-        <v>0.7</v>
-      </c>
+    <row r="52" spans="9:75" x14ac:dyDescent="0.25">
+      <c r="I52" s="125"/>
+      <c r="J52" s="125"/>
+      <c r="K52" s="124"/>
       <c r="AN52" s="19"/>
       <c r="AO52" s="52"/>
       <c r="AP52" s="52"/>
@@ -18335,16 +18294,10 @@
       <c r="BV52" s="52"/>
       <c r="BW52" s="55"/>
     </row>
-    <row r="53" spans="9:75" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="I53" s="125">
-        <v>44305</v>
-      </c>
-      <c r="J53" s="125">
-        <v>44324</v>
-      </c>
-      <c r="K53" s="124">
-        <v>0</v>
-      </c>
+    <row r="53" spans="9:75" x14ac:dyDescent="0.25">
+      <c r="I53" s="125"/>
+      <c r="J53" s="125"/>
+      <c r="K53" s="124"/>
       <c r="AN53" s="19"/>
       <c r="AO53" s="52"/>
       <c r="AP53" s="52"/>
@@ -19942,20 +19895,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B17:B22"/>
     <mergeCell ref="BH5:BK5"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="BT5:BW5"/>
@@ -19971,6 +19910,20 @@
     <mergeCell ref="P5:S5"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="AB5:AE5"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B14"/>
   </mergeCells>
   <conditionalFormatting sqref="K7:R7 K8 L9 M13:M14 N23:U23 V24:X26 L11:L12 C2 M15:O17 T15 T16:Y17 N18:T22 AB15">
     <cfRule type="expression" dxfId="184" priority="178">
@@ -20520,8 +20473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20666,17 +20619,19 @@
       <c r="E10" s="94"/>
       <c r="F10" s="94"/>
       <c r="G10" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="94"/>
+        <v>33</v>
+      </c>
+      <c r="H10" s="94" t="s">
+        <v>136</v>
+      </c>
       <c r="I10" s="104">
         <v>44278</v>
       </c>
       <c r="J10" s="104">
         <v>44310</v>
       </c>
-      <c r="K10" s="111">
-        <v>0.2</v>
+      <c r="K10" s="105">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
@@ -20690,17 +20645,19 @@
       <c r="E11" s="94"/>
       <c r="F11" s="94"/>
       <c r="G11" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="94"/>
+        <v>33</v>
+      </c>
+      <c r="H11" s="94" t="s">
+        <v>136</v>
+      </c>
       <c r="I11" s="104">
         <v>44278</v>
       </c>
       <c r="J11" s="104">
         <v>44310</v>
       </c>
-      <c r="K11" s="111">
-        <v>0.2</v>
+      <c r="K11" s="105">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -21020,8 +20977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21032,7 +20989,7 @@
     <col min="4" max="4" width="17.28515625" style="133" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="132" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" style="132" customWidth="1"/>
-    <col min="7" max="7" width="11" style="132" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="132" customWidth="1"/>
     <col min="8" max="8" width="12.140625" style="132" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="132" customWidth="1"/>
     <col min="10" max="11" width="13.28515625" style="132" customWidth="1"/>
@@ -22094,18 +22051,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="207" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="203">
+      <c r="B3" s="208">
         <v>1</v>
       </c>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="107" t="s">
@@ -22418,7 +22375,7 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22429,18 +22386,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="207" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="203">
+      <c r="B3" s="208">
         <v>2</v>
       </c>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="107" t="s">
@@ -22552,18 +22509,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="207" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="203">
+      <c r="B3" s="208">
         <v>3</v>
       </c>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="107" t="s">
@@ -22664,18 +22621,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="207" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="203">
+      <c r="B3" s="208">
         <v>4</v>
       </c>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="107" t="s">
@@ -22797,8 +22754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22809,18 +22766,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="207" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="203">
+      <c r="B3" s="208">
         <v>5</v>
       </c>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="107" t="s">
@@ -22918,7 +22875,7 @@
         <v>115</v>
       </c>
       <c r="D15" s="94" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -22998,18 +22955,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="207" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="203">
+      <c r="B3" s="208">
         <v>6</v>
       </c>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="107" t="s">

</xml_diff>